<commit_message>
Fixed status in due diligence export
</commit_message>
<xml_diff>
--- a/src/private/templates/suppliers_due_diligence.xlsx
+++ b/src/private/templates/suppliers_due_diligence.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="51200" windowHeight="28260" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17460" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -44,13 +44,13 @@
     <t>Tier type</t>
   </si>
   <si>
-    <t>Prequalification status</t>
-  </si>
-  <si>
     <t>Last report file</t>
   </si>
   <si>
     <t>Expiration date</t>
+  </si>
+  <si>
+    <t>Status</t>
   </si>
 </sst>
 </file>
@@ -367,8 +367,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I1"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="244" zoomScaleNormal="244" zoomScalePageLayoutView="244" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="244" zoomScaleNormal="244" zoomScalePageLayoutView="244" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -392,13 +392,13 @@
         <v>5</v>
       </c>
       <c r="D1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E1" t="s">
         <v>6</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>7</v>
-      </c>
-      <c r="F1" t="s">
-        <v>8</v>
       </c>
       <c r="G1" t="s">
         <v>3</v>

</xml_diff>